<commit_message>
Diagrama de Gantt corregido
</commit_message>
<xml_diff>
--- a/Diagrama De Gantt.xlsx
+++ b/Diagrama De Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Desktop\AnalisisDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1A9BAE-4E95-4D72-AADC-856260E4519B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA368006-BD94-4F0E-903E-7C4D67961FA1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{73C6C5DB-9C78-4B67-932A-CC996DE83013}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Descripción detallada del problema.</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Diagrama de GANTT.</t>
-  </si>
-  <si>
-    <t>Entrevistas.</t>
   </si>
   <si>
     <t>Recopilación de información.</t>
@@ -105,57 +102,6 @@
     <t>Leonardo Miranda</t>
   </si>
   <si>
-    <t>FASE V</t>
-  </si>
-  <si>
-    <t>Instalación de frameworks u IDEs.</t>
-  </si>
-  <si>
-    <t>Maquetación del sistema.</t>
-  </si>
-  <si>
-    <t>Realización del manual de usuario.</t>
-  </si>
-  <si>
-    <t>Conexión del sistema con la base de datos.</t>
-  </si>
-  <si>
-    <t>Creación de la base de datos del sistema.</t>
-  </si>
-  <si>
-    <t>FASE VI</t>
-  </si>
-  <si>
-    <t>Pruebas unitarias.</t>
-  </si>
-  <si>
-    <t>Pruebas de integración.</t>
-  </si>
-  <si>
-    <t>Pruebas de aceptación.</t>
-  </si>
-  <si>
-    <t>Pruebas Alpha.</t>
-  </si>
-  <si>
-    <t>Pruebas Beta.</t>
-  </si>
-  <si>
-    <t>Pruebas de regresión.</t>
-  </si>
-  <si>
-    <t>Pruebas de humo.</t>
-  </si>
-  <si>
-    <t>FASE VII</t>
-  </si>
-  <si>
-    <t>Implentación del sistema.</t>
-  </si>
-  <si>
-    <t>Documentación.</t>
-  </si>
-  <si>
     <t>Todos</t>
   </si>
   <si>
@@ -174,22 +120,13 @@
     <t>RESPONSABLE</t>
   </si>
   <si>
-    <t>ACOTACIONES</t>
-  </si>
-  <si>
-    <t>DONE</t>
-  </si>
-  <si>
-    <t>DOING</t>
-  </si>
-  <si>
-    <t>TO DO</t>
-  </si>
-  <si>
     <t>Objetivo general y especificos.</t>
   </si>
   <si>
     <t>Objetivos de producto y proyecto.</t>
+  </si>
+  <si>
+    <t>Documentacion</t>
   </si>
 </sst>
 </file>
@@ -228,7 +165,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,24 +216,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -424,11 +355,78 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -450,22 +448,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -478,24 +474,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -510,37 +503,52 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -871,7 +879,7 @@
   <dimension ref="A1:DI162"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C6"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,96 +958,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:113" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="36" t="s">
-        <v>42</v>
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="11" t="s">
+        <v>24</v>
       </c>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="37"/>
-      <c r="AD1" s="37"/>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="37"/>
-      <c r="AG1" s="37"/>
-      <c r="AH1" s="38"/>
-      <c r="AI1" s="36" t="s">
-        <v>43</v>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="13"/>
+      <c r="AI1" s="11" t="s">
+        <v>25</v>
       </c>
-      <c r="AJ1" s="37"/>
-      <c r="AK1" s="37"/>
-      <c r="AL1" s="37"/>
-      <c r="AM1" s="37"/>
-      <c r="AN1" s="37"/>
-      <c r="AO1" s="37"/>
-      <c r="AP1" s="37"/>
-      <c r="AQ1" s="37"/>
-      <c r="AR1" s="37"/>
-      <c r="AS1" s="37"/>
-      <c r="AT1" s="37"/>
-      <c r="AU1" s="37"/>
-      <c r="AV1" s="37"/>
-      <c r="AW1" s="37"/>
-      <c r="AX1" s="37"/>
-      <c r="AY1" s="37"/>
-      <c r="AZ1" s="37"/>
-      <c r="BA1" s="37"/>
-      <c r="BB1" s="37"/>
-      <c r="BC1" s="37"/>
-      <c r="BD1" s="37"/>
-      <c r="BE1" s="37"/>
-      <c r="BF1" s="37"/>
-      <c r="BG1" s="37"/>
-      <c r="BH1" s="37"/>
-      <c r="BI1" s="37"/>
-      <c r="BJ1" s="37"/>
-      <c r="BK1" s="37"/>
-      <c r="BL1" s="37"/>
-      <c r="BM1" s="38"/>
-      <c r="BN1" s="36" t="s">
-        <v>44</v>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="12"/>
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="12"/>
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="12"/>
+      <c r="AU1" s="12"/>
+      <c r="AV1" s="12"/>
+      <c r="AW1" s="12"/>
+      <c r="AX1" s="12"/>
+      <c r="AY1" s="12"/>
+      <c r="AZ1" s="12"/>
+      <c r="BA1" s="12"/>
+      <c r="BB1" s="12"/>
+      <c r="BC1" s="12"/>
+      <c r="BD1" s="12"/>
+      <c r="BE1" s="12"/>
+      <c r="BF1" s="12"/>
+      <c r="BG1" s="12"/>
+      <c r="BH1" s="12"/>
+      <c r="BI1" s="12"/>
+      <c r="BJ1" s="12"/>
+      <c r="BK1" s="12"/>
+      <c r="BL1" s="12"/>
+      <c r="BM1" s="13"/>
+      <c r="BN1" s="11" t="s">
+        <v>26</v>
       </c>
-      <c r="BO1" s="37"/>
-      <c r="BP1" s="37"/>
-      <c r="BQ1" s="37"/>
-      <c r="BR1" s="37"/>
-      <c r="BS1" s="37"/>
-      <c r="BT1" s="37"/>
-      <c r="BU1" s="37"/>
-      <c r="BV1" s="37"/>
-      <c r="BW1" s="37"/>
-      <c r="BX1" s="37"/>
-      <c r="BY1" s="37"/>
-      <c r="BZ1" s="37"/>
-      <c r="CA1" s="37"/>
-      <c r="CB1" s="37"/>
-      <c r="CC1" s="37"/>
-      <c r="CD1" s="37"/>
-      <c r="CE1" s="37"/>
-      <c r="CF1" s="38"/>
+      <c r="BO1" s="12"/>
+      <c r="BP1" s="12"/>
+      <c r="BQ1" s="12"/>
+      <c r="BR1" s="12"/>
+      <c r="BS1" s="12"/>
+      <c r="BT1" s="12"/>
+      <c r="BU1" s="12"/>
+      <c r="BV1" s="12"/>
+      <c r="BW1" s="12"/>
+      <c r="BX1" s="12"/>
+      <c r="BY1" s="12"/>
+      <c r="BZ1" s="12"/>
+      <c r="CA1" s="12"/>
+      <c r="CB1" s="12"/>
+      <c r="CC1" s="12"/>
+      <c r="CD1" s="12"/>
+      <c r="CE1" s="12"/>
+      <c r="CF1" s="13"/>
       <c r="CG1" s="6"/>
       <c r="CH1" s="6"/>
       <c r="CI1" s="6"/>
@@ -1069,14 +1077,14 @@
       <c r="DG1" s="6"/>
     </row>
     <row r="2" spans="1:113" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
-        <v>19</v>
+      <c r="A2" s="25" t="s">
+        <v>18</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
       <c r="G2" s="2">
         <v>3</v>
       </c>
@@ -1340,18 +1348,18 @@
       <c r="DG2" s="6"/>
     </row>
     <row r="3" spans="1:113" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
-        <v>7</v>
+      <c r="A3" s="19" t="s">
+        <v>6</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="33"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="21"/>
       <c r="D3" s="5" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
-      <c r="E3" s="34" t="s">
-        <v>46</v>
+      <c r="E3" s="28" t="s">
+        <v>28</v>
       </c>
-      <c r="F3" s="35"/>
+      <c r="F3" s="29"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -1461,96 +1469,96 @@
       <c r="DI3" s="1"/>
     </row>
     <row r="4" spans="1:113" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="3">
         <v>2</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>20</v>
+      <c r="E4" s="15" t="s">
+        <v>19</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="20"/>
-      <c r="U4" s="20"/>
-      <c r="V4" s="20"/>
-      <c r="W4" s="20"/>
-      <c r="X4" s="20"/>
-      <c r="Y4" s="20"/>
-      <c r="Z4" s="20"/>
-      <c r="AA4" s="20"/>
-      <c r="AB4" s="20"/>
-      <c r="AC4" s="20"/>
-      <c r="AD4" s="20"/>
-      <c r="AE4" s="20"/>
-      <c r="AF4" s="20"/>
-      <c r="AG4" s="20"/>
-      <c r="AH4" s="20"/>
-      <c r="AI4" s="20"/>
-      <c r="AJ4" s="20"/>
-      <c r="AK4" s="20"/>
-      <c r="AL4" s="20"/>
-      <c r="AM4" s="20"/>
-      <c r="AN4" s="20"/>
-      <c r="AO4" s="20"/>
-      <c r="AP4" s="20"/>
-      <c r="AQ4" s="20"/>
-      <c r="AR4" s="20"/>
-      <c r="AS4" s="20"/>
-      <c r="AT4" s="20"/>
-      <c r="AU4" s="20"/>
-      <c r="AV4" s="20"/>
-      <c r="AW4" s="20"/>
-      <c r="AX4" s="20"/>
-      <c r="AY4" s="20"/>
-      <c r="AZ4" s="20"/>
-      <c r="BA4" s="20"/>
-      <c r="BB4" s="20"/>
-      <c r="BC4" s="20"/>
-      <c r="BD4" s="20"/>
-      <c r="BE4" s="20"/>
-      <c r="BF4" s="20"/>
-      <c r="BG4" s="20"/>
-      <c r="BH4" s="20"/>
-      <c r="BI4" s="20"/>
-      <c r="BJ4" s="20"/>
-      <c r="BK4" s="20"/>
-      <c r="BL4" s="20"/>
-      <c r="BM4" s="20"/>
-      <c r="BN4" s="20"/>
-      <c r="BO4" s="20"/>
-      <c r="BP4" s="20"/>
-      <c r="BQ4" s="20"/>
-      <c r="BR4" s="20"/>
-      <c r="BS4" s="20"/>
-      <c r="BT4" s="20"/>
-      <c r="BU4" s="20"/>
-      <c r="BV4" s="20"/>
-      <c r="BW4" s="20"/>
-      <c r="BX4" s="20"/>
-      <c r="BY4" s="20"/>
-      <c r="BZ4" s="20"/>
-      <c r="CA4" s="20"/>
-      <c r="CB4" s="20"/>
-      <c r="CC4" s="20"/>
-      <c r="CD4" s="20"/>
-      <c r="CE4" s="20"/>
-      <c r="CF4" s="20"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="10"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="10"/>
+      <c r="AE4" s="10"/>
+      <c r="AF4" s="10"/>
+      <c r="AG4" s="10"/>
+      <c r="AH4" s="10"/>
+      <c r="AI4" s="10"/>
+      <c r="AJ4" s="10"/>
+      <c r="AK4" s="10"/>
+      <c r="AL4" s="10"/>
+      <c r="AM4" s="10"/>
+      <c r="AN4" s="10"/>
+      <c r="AO4" s="10"/>
+      <c r="AP4" s="10"/>
+      <c r="AQ4" s="10"/>
+      <c r="AR4" s="10"/>
+      <c r="AS4" s="10"/>
+      <c r="AT4" s="10"/>
+      <c r="AU4" s="10"/>
+      <c r="AV4" s="10"/>
+      <c r="AW4" s="10"/>
+      <c r="AX4" s="10"/>
+      <c r="AY4" s="10"/>
+      <c r="AZ4" s="10"/>
+      <c r="BA4" s="10"/>
+      <c r="BB4" s="10"/>
+      <c r="BC4" s="10"/>
+      <c r="BD4" s="10"/>
+      <c r="BE4" s="10"/>
+      <c r="BF4" s="10"/>
+      <c r="BG4" s="10"/>
+      <c r="BH4" s="10"/>
+      <c r="BI4" s="10"/>
+      <c r="BJ4" s="10"/>
+      <c r="BK4" s="10"/>
+      <c r="BL4" s="10"/>
+      <c r="BM4" s="10"/>
+      <c r="BN4" s="10"/>
+      <c r="BO4" s="10"/>
+      <c r="BP4" s="10"/>
+      <c r="BQ4" s="10"/>
+      <c r="BR4" s="10"/>
+      <c r="BS4" s="10"/>
+      <c r="BT4" s="10"/>
+      <c r="BU4" s="10"/>
+      <c r="BV4" s="10"/>
+      <c r="BW4" s="10"/>
+      <c r="BX4" s="10"/>
+      <c r="BY4" s="10"/>
+      <c r="BZ4" s="10"/>
+      <c r="CA4" s="10"/>
+      <c r="CB4" s="10"/>
+      <c r="CC4" s="10"/>
+      <c r="CD4" s="10"/>
+      <c r="CE4" s="10"/>
+      <c r="CF4" s="10"/>
       <c r="CG4" s="6"/>
       <c r="CH4" s="6"/>
       <c r="CI4" s="6"/>
@@ -1580,96 +1588,96 @@
       <c r="DG4" s="6"/>
     </row>
     <row r="5" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>51</v>
+      <c r="A5" s="15" t="s">
+        <v>29</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="3">
         <v>2</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>20</v>
+      <c r="E5" s="15" t="s">
+        <v>19</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="20"/>
-      <c r="U5" s="20"/>
-      <c r="V5" s="20"/>
-      <c r="W5" s="20"/>
-      <c r="X5" s="20"/>
-      <c r="Y5" s="20"/>
-      <c r="Z5" s="20"/>
-      <c r="AA5" s="20"/>
-      <c r="AB5" s="20"/>
-      <c r="AC5" s="20"/>
-      <c r="AD5" s="20"/>
-      <c r="AE5" s="20"/>
-      <c r="AF5" s="20"/>
-      <c r="AG5" s="20"/>
-      <c r="AH5" s="20"/>
-      <c r="AI5" s="20"/>
-      <c r="AJ5" s="20"/>
-      <c r="AK5" s="20"/>
-      <c r="AL5" s="20"/>
-      <c r="AM5" s="20"/>
-      <c r="AN5" s="20"/>
-      <c r="AO5" s="20"/>
-      <c r="AP5" s="20"/>
-      <c r="AQ5" s="20"/>
-      <c r="AR5" s="20"/>
-      <c r="AS5" s="20"/>
-      <c r="AT5" s="20"/>
-      <c r="AU5" s="20"/>
-      <c r="AV5" s="20"/>
-      <c r="AW5" s="20"/>
-      <c r="AX5" s="20"/>
-      <c r="AY5" s="20"/>
-      <c r="AZ5" s="20"/>
-      <c r="BA5" s="20"/>
-      <c r="BB5" s="20"/>
-      <c r="BC5" s="20"/>
-      <c r="BD5" s="20"/>
-      <c r="BE5" s="20"/>
-      <c r="BF5" s="20"/>
-      <c r="BG5" s="20"/>
-      <c r="BH5" s="20"/>
-      <c r="BI5" s="20"/>
-      <c r="BJ5" s="20"/>
-      <c r="BK5" s="20"/>
-      <c r="BL5" s="20"/>
-      <c r="BM5" s="20"/>
-      <c r="BN5" s="20"/>
-      <c r="BO5" s="20"/>
-      <c r="BP5" s="20"/>
-      <c r="BQ5" s="20"/>
-      <c r="BR5" s="20"/>
-      <c r="BS5" s="20"/>
-      <c r="BT5" s="20"/>
-      <c r="BU5" s="20"/>
-      <c r="BV5" s="20"/>
-      <c r="BW5" s="20"/>
-      <c r="BX5" s="20"/>
-      <c r="BY5" s="20"/>
-      <c r="BZ5" s="20"/>
-      <c r="CA5" s="20"/>
-      <c r="CB5" s="20"/>
-      <c r="CC5" s="20"/>
-      <c r="CD5" s="20"/>
-      <c r="CE5" s="20"/>
-      <c r="CF5" s="20"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="10"/>
+      <c r="AH5" s="10"/>
+      <c r="AI5" s="10"/>
+      <c r="AJ5" s="10"/>
+      <c r="AK5" s="10"/>
+      <c r="AL5" s="10"/>
+      <c r="AM5" s="10"/>
+      <c r="AN5" s="10"/>
+      <c r="AO5" s="10"/>
+      <c r="AP5" s="10"/>
+      <c r="AQ5" s="10"/>
+      <c r="AR5" s="10"/>
+      <c r="AS5" s="10"/>
+      <c r="AT5" s="10"/>
+      <c r="AU5" s="10"/>
+      <c r="AV5" s="10"/>
+      <c r="AW5" s="10"/>
+      <c r="AX5" s="10"/>
+      <c r="AY5" s="10"/>
+      <c r="AZ5" s="10"/>
+      <c r="BA5" s="10"/>
+      <c r="BB5" s="10"/>
+      <c r="BC5" s="10"/>
+      <c r="BD5" s="10"/>
+      <c r="BE5" s="10"/>
+      <c r="BF5" s="10"/>
+      <c r="BG5" s="10"/>
+      <c r="BH5" s="10"/>
+      <c r="BI5" s="10"/>
+      <c r="BJ5" s="10"/>
+      <c r="BK5" s="10"/>
+      <c r="BL5" s="10"/>
+      <c r="BM5" s="10"/>
+      <c r="BN5" s="10"/>
+      <c r="BO5" s="10"/>
+      <c r="BP5" s="10"/>
+      <c r="BQ5" s="10"/>
+      <c r="BR5" s="10"/>
+      <c r="BS5" s="10"/>
+      <c r="BT5" s="10"/>
+      <c r="BU5" s="10"/>
+      <c r="BV5" s="10"/>
+      <c r="BW5" s="10"/>
+      <c r="BX5" s="10"/>
+      <c r="BY5" s="10"/>
+      <c r="BZ5" s="10"/>
+      <c r="CA5" s="10"/>
+      <c r="CB5" s="10"/>
+      <c r="CC5" s="10"/>
+      <c r="CD5" s="10"/>
+      <c r="CE5" s="10"/>
+      <c r="CF5" s="10"/>
       <c r="CG5" s="6"/>
       <c r="CH5" s="6"/>
       <c r="CI5" s="6"/>
@@ -1699,96 +1707,96 @@
       <c r="DG5" s="6"/>
     </row>
     <row r="6" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>52</v>
+      <c r="A6" s="15" t="s">
+        <v>30</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="3">
         <v>2</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>20</v>
+      <c r="E6" s="15" t="s">
+        <v>19</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="20"/>
-      <c r="S6" s="20"/>
-      <c r="T6" s="20"/>
-      <c r="U6" s="20"/>
-      <c r="V6" s="20"/>
-      <c r="W6" s="20"/>
-      <c r="X6" s="20"/>
-      <c r="Y6" s="20"/>
-      <c r="Z6" s="20"/>
-      <c r="AA6" s="20"/>
-      <c r="AB6" s="20"/>
-      <c r="AC6" s="20"/>
-      <c r="AD6" s="20"/>
-      <c r="AE6" s="20"/>
-      <c r="AF6" s="20"/>
-      <c r="AG6" s="20"/>
-      <c r="AH6" s="20"/>
-      <c r="AI6" s="20"/>
-      <c r="AJ6" s="20"/>
-      <c r="AK6" s="20"/>
-      <c r="AL6" s="20"/>
-      <c r="AM6" s="20"/>
-      <c r="AN6" s="20"/>
-      <c r="AO6" s="20"/>
-      <c r="AP6" s="20"/>
-      <c r="AQ6" s="20"/>
-      <c r="AR6" s="20"/>
-      <c r="AS6" s="20"/>
-      <c r="AT6" s="20"/>
-      <c r="AU6" s="20"/>
-      <c r="AV6" s="20"/>
-      <c r="AW6" s="20"/>
-      <c r="AX6" s="20"/>
-      <c r="AY6" s="20"/>
-      <c r="AZ6" s="20"/>
-      <c r="BA6" s="20"/>
-      <c r="BB6" s="20"/>
-      <c r="BC6" s="20"/>
-      <c r="BD6" s="20"/>
-      <c r="BE6" s="20"/>
-      <c r="BF6" s="20"/>
-      <c r="BG6" s="20"/>
-      <c r="BH6" s="20"/>
-      <c r="BI6" s="20"/>
-      <c r="BJ6" s="20"/>
-      <c r="BK6" s="20"/>
-      <c r="BL6" s="20"/>
-      <c r="BM6" s="20"/>
-      <c r="BN6" s="20"/>
-      <c r="BO6" s="20"/>
-      <c r="BP6" s="20"/>
-      <c r="BQ6" s="20"/>
-      <c r="BR6" s="20"/>
-      <c r="BS6" s="20"/>
-      <c r="BT6" s="20"/>
-      <c r="BU6" s="20"/>
-      <c r="BV6" s="20"/>
-      <c r="BW6" s="20"/>
-      <c r="BX6" s="20"/>
-      <c r="BY6" s="20"/>
-      <c r="BZ6" s="20"/>
-      <c r="CA6" s="20"/>
-      <c r="CB6" s="20"/>
-      <c r="CC6" s="20"/>
-      <c r="CD6" s="20"/>
-      <c r="CE6" s="20"/>
-      <c r="CF6" s="20"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="10"/>
+      <c r="AB6" s="10"/>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="10"/>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="10"/>
+      <c r="AI6" s="10"/>
+      <c r="AJ6" s="10"/>
+      <c r="AK6" s="10"/>
+      <c r="AL6" s="10"/>
+      <c r="AM6" s="10"/>
+      <c r="AN6" s="10"/>
+      <c r="AO6" s="10"/>
+      <c r="AP6" s="10"/>
+      <c r="AQ6" s="10"/>
+      <c r="AR6" s="10"/>
+      <c r="AS6" s="10"/>
+      <c r="AT6" s="10"/>
+      <c r="AU6" s="10"/>
+      <c r="AV6" s="10"/>
+      <c r="AW6" s="10"/>
+      <c r="AX6" s="10"/>
+      <c r="AY6" s="10"/>
+      <c r="AZ6" s="10"/>
+      <c r="BA6" s="10"/>
+      <c r="BB6" s="10"/>
+      <c r="BC6" s="10"/>
+      <c r="BD6" s="10"/>
+      <c r="BE6" s="10"/>
+      <c r="BF6" s="10"/>
+      <c r="BG6" s="10"/>
+      <c r="BH6" s="10"/>
+      <c r="BI6" s="10"/>
+      <c r="BJ6" s="10"/>
+      <c r="BK6" s="10"/>
+      <c r="BL6" s="10"/>
+      <c r="BM6" s="10"/>
+      <c r="BN6" s="10"/>
+      <c r="BO6" s="10"/>
+      <c r="BP6" s="10"/>
+      <c r="BQ6" s="10"/>
+      <c r="BR6" s="10"/>
+      <c r="BS6" s="10"/>
+      <c r="BT6" s="10"/>
+      <c r="BU6" s="10"/>
+      <c r="BV6" s="10"/>
+      <c r="BW6" s="10"/>
+      <c r="BX6" s="10"/>
+      <c r="BY6" s="10"/>
+      <c r="BZ6" s="10"/>
+      <c r="CA6" s="10"/>
+      <c r="CB6" s="10"/>
+      <c r="CC6" s="10"/>
+      <c r="CD6" s="10"/>
+      <c r="CE6" s="10"/>
+      <c r="CF6" s="10"/>
       <c r="CG6" s="6"/>
       <c r="CH6" s="6"/>
       <c r="CI6" s="6"/>
@@ -1818,96 +1826,96 @@
       <c r="DG6" s="6"/>
     </row>
     <row r="7" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="3">
         <v>3</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>21</v>
+      <c r="E7" s="15" t="s">
+        <v>20</v>
       </c>
-      <c r="F7" s="19"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="20"/>
-      <c r="S7" s="20"/>
-      <c r="T7" s="20"/>
-      <c r="U7" s="20"/>
-      <c r="V7" s="20"/>
-      <c r="W7" s="20"/>
-      <c r="X7" s="20"/>
-      <c r="Y7" s="20"/>
-      <c r="Z7" s="20"/>
-      <c r="AA7" s="20"/>
-      <c r="AB7" s="20"/>
-      <c r="AC7" s="20"/>
-      <c r="AD7" s="20"/>
-      <c r="AE7" s="20"/>
-      <c r="AF7" s="20"/>
-      <c r="AG7" s="20"/>
-      <c r="AH7" s="20"/>
-      <c r="AI7" s="20"/>
-      <c r="AJ7" s="20"/>
-      <c r="AK7" s="20"/>
-      <c r="AL7" s="20"/>
-      <c r="AM7" s="20"/>
-      <c r="AN7" s="20"/>
-      <c r="AO7" s="20"/>
-      <c r="AP7" s="20"/>
-      <c r="AQ7" s="20"/>
-      <c r="AR7" s="20"/>
-      <c r="AS7" s="20"/>
-      <c r="AT7" s="20"/>
-      <c r="AU7" s="20"/>
-      <c r="AV7" s="20"/>
-      <c r="AW7" s="20"/>
-      <c r="AX7" s="20"/>
-      <c r="AY7" s="20"/>
-      <c r="AZ7" s="20"/>
-      <c r="BA7" s="20"/>
-      <c r="BB7" s="20"/>
-      <c r="BC7" s="20"/>
-      <c r="BD7" s="20"/>
-      <c r="BE7" s="20"/>
-      <c r="BF7" s="20"/>
-      <c r="BG7" s="20"/>
-      <c r="BH7" s="20"/>
-      <c r="BI7" s="20"/>
-      <c r="BJ7" s="20"/>
-      <c r="BK7" s="20"/>
-      <c r="BL7" s="20"/>
-      <c r="BM7" s="20"/>
-      <c r="BN7" s="20"/>
-      <c r="BO7" s="20"/>
-      <c r="BP7" s="20"/>
-      <c r="BQ7" s="20"/>
-      <c r="BR7" s="20"/>
-      <c r="BS7" s="20"/>
-      <c r="BT7" s="20"/>
-      <c r="BU7" s="20"/>
-      <c r="BV7" s="20"/>
-      <c r="BW7" s="20"/>
-      <c r="BX7" s="20"/>
-      <c r="BY7" s="20"/>
-      <c r="BZ7" s="20"/>
-      <c r="CA7" s="20"/>
-      <c r="CB7" s="20"/>
-      <c r="CC7" s="20"/>
-      <c r="CD7" s="20"/>
-      <c r="CE7" s="20"/>
-      <c r="CF7" s="20"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="10"/>
+      <c r="AE7" s="10"/>
+      <c r="AF7" s="10"/>
+      <c r="AG7" s="10"/>
+      <c r="AH7" s="10"/>
+      <c r="AI7" s="10"/>
+      <c r="AJ7" s="10"/>
+      <c r="AK7" s="10"/>
+      <c r="AL7" s="10"/>
+      <c r="AM7" s="10"/>
+      <c r="AN7" s="10"/>
+      <c r="AO7" s="10"/>
+      <c r="AP7" s="10"/>
+      <c r="AQ7" s="10"/>
+      <c r="AR7" s="10"/>
+      <c r="AS7" s="10"/>
+      <c r="AT7" s="10"/>
+      <c r="AU7" s="10"/>
+      <c r="AV7" s="10"/>
+      <c r="AW7" s="10"/>
+      <c r="AX7" s="10"/>
+      <c r="AY7" s="10"/>
+      <c r="AZ7" s="10"/>
+      <c r="BA7" s="10"/>
+      <c r="BB7" s="10"/>
+      <c r="BC7" s="10"/>
+      <c r="BD7" s="10"/>
+      <c r="BE7" s="10"/>
+      <c r="BF7" s="10"/>
+      <c r="BG7" s="10"/>
+      <c r="BH7" s="10"/>
+      <c r="BI7" s="10"/>
+      <c r="BJ7" s="10"/>
+      <c r="BK7" s="10"/>
+      <c r="BL7" s="10"/>
+      <c r="BM7" s="10"/>
+      <c r="BN7" s="10"/>
+      <c r="BO7" s="10"/>
+      <c r="BP7" s="10"/>
+      <c r="BQ7" s="10"/>
+      <c r="BR7" s="10"/>
+      <c r="BS7" s="10"/>
+      <c r="BT7" s="10"/>
+      <c r="BU7" s="10"/>
+      <c r="BV7" s="10"/>
+      <c r="BW7" s="10"/>
+      <c r="BX7" s="10"/>
+      <c r="BY7" s="10"/>
+      <c r="BZ7" s="10"/>
+      <c r="CA7" s="10"/>
+      <c r="CB7" s="10"/>
+      <c r="CC7" s="10"/>
+      <c r="CD7" s="10"/>
+      <c r="CE7" s="10"/>
+      <c r="CF7" s="10"/>
       <c r="CG7" s="6"/>
       <c r="CH7" s="6"/>
       <c r="CI7" s="6"/>
@@ -1937,96 +1945,96 @@
       <c r="DG7" s="6"/>
     </row>
     <row r="8" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="3">
         <v>3</v>
       </c>
-      <c r="E8" s="17" t="s">
-        <v>22</v>
+      <c r="E8" s="15" t="s">
+        <v>21</v>
       </c>
-      <c r="F8" s="19"/>
+      <c r="F8" s="17"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="20"/>
-      <c r="U8" s="20"/>
-      <c r="V8" s="20"/>
-      <c r="W8" s="20"/>
-      <c r="X8" s="20"/>
-      <c r="Y8" s="20"/>
-      <c r="Z8" s="20"/>
-      <c r="AA8" s="20"/>
-      <c r="AB8" s="20"/>
-      <c r="AC8" s="20"/>
-      <c r="AD8" s="20"/>
-      <c r="AE8" s="20"/>
-      <c r="AF8" s="20"/>
-      <c r="AG8" s="20"/>
-      <c r="AH8" s="20"/>
-      <c r="AI8" s="20"/>
-      <c r="AJ8" s="20"/>
-      <c r="AK8" s="20"/>
-      <c r="AL8" s="20"/>
-      <c r="AM8" s="20"/>
-      <c r="AN8" s="20"/>
-      <c r="AO8" s="20"/>
-      <c r="AP8" s="20"/>
-      <c r="AQ8" s="20"/>
-      <c r="AR8" s="20"/>
-      <c r="AS8" s="20"/>
-      <c r="AT8" s="20"/>
-      <c r="AU8" s="20"/>
-      <c r="AV8" s="20"/>
-      <c r="AW8" s="20"/>
-      <c r="AX8" s="20"/>
-      <c r="AY8" s="20"/>
-      <c r="AZ8" s="20"/>
-      <c r="BA8" s="20"/>
-      <c r="BB8" s="20"/>
-      <c r="BC8" s="20"/>
-      <c r="BD8" s="20"/>
-      <c r="BE8" s="20"/>
-      <c r="BF8" s="20"/>
-      <c r="BG8" s="20"/>
-      <c r="BH8" s="20"/>
-      <c r="BI8" s="20"/>
-      <c r="BJ8" s="20"/>
-      <c r="BK8" s="20"/>
-      <c r="BL8" s="20"/>
-      <c r="BM8" s="20"/>
-      <c r="BN8" s="20"/>
-      <c r="BO8" s="20"/>
-      <c r="BP8" s="20"/>
-      <c r="BQ8" s="20"/>
-      <c r="BR8" s="20"/>
-      <c r="BS8" s="20"/>
-      <c r="BT8" s="20"/>
-      <c r="BU8" s="20"/>
-      <c r="BV8" s="20"/>
-      <c r="BW8" s="20"/>
-      <c r="BX8" s="20"/>
-      <c r="BY8" s="20"/>
-      <c r="BZ8" s="20"/>
-      <c r="CA8" s="20"/>
-      <c r="CB8" s="20"/>
-      <c r="CC8" s="20"/>
-      <c r="CD8" s="20"/>
-      <c r="CE8" s="20"/>
-      <c r="CF8" s="20"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="10"/>
+      <c r="AB8" s="10"/>
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="10"/>
+      <c r="AE8" s="10"/>
+      <c r="AF8" s="10"/>
+      <c r="AG8" s="10"/>
+      <c r="AH8" s="10"/>
+      <c r="AI8" s="10"/>
+      <c r="AJ8" s="10"/>
+      <c r="AK8" s="10"/>
+      <c r="AL8" s="10"/>
+      <c r="AM8" s="10"/>
+      <c r="AN8" s="10"/>
+      <c r="AO8" s="10"/>
+      <c r="AP8" s="10"/>
+      <c r="AQ8" s="10"/>
+      <c r="AR8" s="10"/>
+      <c r="AS8" s="10"/>
+      <c r="AT8" s="10"/>
+      <c r="AU8" s="10"/>
+      <c r="AV8" s="10"/>
+      <c r="AW8" s="10"/>
+      <c r="AX8" s="10"/>
+      <c r="AY8" s="10"/>
+      <c r="AZ8" s="10"/>
+      <c r="BA8" s="10"/>
+      <c r="BB8" s="10"/>
+      <c r="BC8" s="10"/>
+      <c r="BD8" s="10"/>
+      <c r="BE8" s="10"/>
+      <c r="BF8" s="10"/>
+      <c r="BG8" s="10"/>
+      <c r="BH8" s="10"/>
+      <c r="BI8" s="10"/>
+      <c r="BJ8" s="10"/>
+      <c r="BK8" s="10"/>
+      <c r="BL8" s="10"/>
+      <c r="BM8" s="10"/>
+      <c r="BN8" s="10"/>
+      <c r="BO8" s="10"/>
+      <c r="BP8" s="10"/>
+      <c r="BQ8" s="10"/>
+      <c r="BR8" s="10"/>
+      <c r="BS8" s="10"/>
+      <c r="BT8" s="10"/>
+      <c r="BU8" s="10"/>
+      <c r="BV8" s="10"/>
+      <c r="BW8" s="10"/>
+      <c r="BX8" s="10"/>
+      <c r="BY8" s="10"/>
+      <c r="BZ8" s="10"/>
+      <c r="CA8" s="10"/>
+      <c r="CB8" s="10"/>
+      <c r="CC8" s="10"/>
+      <c r="CD8" s="10"/>
+      <c r="CE8" s="10"/>
+      <c r="CF8" s="10"/>
       <c r="CG8" s="6"/>
       <c r="CH8" s="6"/>
       <c r="CI8" s="6"/>
@@ -2056,9 +2064,9 @@
       <c r="DG8" s="6"/>
     </row>
     <row r="9" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -2169,11 +2177,11 @@
       <c r="DG9" s="6"/>
     </row>
     <row r="10" spans="1:113" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
-        <v>8</v>
+      <c r="A10" s="19" t="s">
+        <v>7</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="33"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -2284,18 +2292,18 @@
       <c r="DG10" s="6"/>
     </row>
     <row r="11" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>4</v>
+      <c r="A11" s="35" t="s">
+        <v>3</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="3">
+      <c r="B11" s="36"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="38">
         <v>7</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>22</v>
+      <c r="E11" s="35" t="s">
+        <v>21</v>
       </c>
-      <c r="F11" s="19"/>
+      <c r="F11" s="37"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -2305,13 +2313,13 @@
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="32"/>
+      <c r="T11" s="32"/>
+      <c r="U11" s="32"/>
+      <c r="V11" s="32"/>
       <c r="W11" s="6"/>
       <c r="X11" s="6"/>
       <c r="Y11" s="6"/>
@@ -2403,18 +2411,12 @@
       <c r="DG11" s="6"/>
     </row>
     <row r="12" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="3">
-        <v>7</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="19"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2424,13 +2426,13 @@
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
-      <c r="V12" s="15"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
       <c r="W12" s="6"/>
       <c r="X12" s="6"/>
       <c r="Y12" s="6"/>
@@ -2522,9 +2524,9 @@
       <c r="DG12" s="6"/>
     </row>
     <row r="13" spans="1:113" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -2635,11 +2637,11 @@
       <c r="DG13" s="6"/>
     </row>
     <row r="14" spans="1:113" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
-        <v>9</v>
+      <c r="A14" s="19" t="s">
+        <v>8</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="33"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="21"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -2750,18 +2752,18 @@
       <c r="DG14" s="6"/>
     </row>
     <row r="15" spans="1:113" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>6</v>
+      <c r="A15" s="15" t="s">
+        <v>5</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
       <c r="D15" s="3">
         <v>6</v>
       </c>
-      <c r="E15" s="21" t="s">
-        <v>23</v>
+      <c r="E15" s="30" t="s">
+        <v>22</v>
       </c>
-      <c r="F15" s="22"/>
+      <c r="F15" s="31"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
@@ -2772,12 +2774,12 @@
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
+      <c r="Q15" s="32"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="32"/>
+      <c r="T15" s="32"/>
+      <c r="U15" s="32"/>
+      <c r="V15" s="32"/>
       <c r="W15" s="6"/>
       <c r="X15" s="6"/>
       <c r="Y15" s="6"/>
@@ -2869,18 +2871,18 @@
       <c r="DG15" s="6"/>
     </row>
     <row r="16" spans="1:113" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>5</v>
+      <c r="A16" s="15" t="s">
+        <v>4</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="3">
         <v>6</v>
       </c>
-      <c r="E16" s="17" t="s">
-        <v>23</v>
+      <c r="E16" s="15" t="s">
+        <v>22</v>
       </c>
-      <c r="F16" s="19"/>
+      <c r="F16" s="17"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -2891,12 +2893,12 @@
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="32"/>
+      <c r="T16" s="32"/>
+      <c r="U16" s="32"/>
+      <c r="V16" s="32"/>
       <c r="W16" s="6"/>
       <c r="X16" s="6"/>
       <c r="Y16" s="6"/>
@@ -2988,9 +2990,9 @@
       <c r="DG16" s="6"/>
     </row>
     <row r="17" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -3101,11 +3103,11 @@
       <c r="DG17" s="6"/>
     </row>
     <row r="18" spans="1:111" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
-        <v>10</v>
+      <c r="A18" s="19" t="s">
+        <v>9</v>
       </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="33"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="21"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -3216,18 +3218,18 @@
       <c r="DG18" s="6"/>
     </row>
     <row r="19" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>11</v>
+      <c r="A19" s="15" t="s">
+        <v>10</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
       <c r="D19" s="3">
         <v>5</v>
       </c>
-      <c r="E19" s="17" t="s">
-        <v>21</v>
+      <c r="E19" s="15" t="s">
+        <v>20</v>
       </c>
-      <c r="F19" s="19"/>
+      <c r="F19" s="17"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
@@ -3235,21 +3237,21 @@
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="16"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
-      <c r="V19" s="6"/>
-      <c r="W19" s="6"/>
-      <c r="X19" s="6"/>
-      <c r="Y19" s="6"/>
-      <c r="Z19" s="6"/>
-      <c r="AA19" s="6"/>
-      <c r="AB19" s="6"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="9"/>
+      <c r="AB19" s="9"/>
       <c r="AC19" s="6"/>
       <c r="AD19" s="6"/>
       <c r="AE19" s="6"/>
@@ -3335,18 +3337,18 @@
       <c r="DG19" s="6"/>
     </row>
     <row r="20" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
-        <v>12</v>
+      <c r="A20" s="15" t="s">
+        <v>11</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
       <c r="D20" s="3">
         <v>5</v>
       </c>
-      <c r="E20" s="17" t="s">
-        <v>20</v>
+      <c r="E20" s="15" t="s">
+        <v>19</v>
       </c>
-      <c r="F20" s="19"/>
+      <c r="F20" s="17"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -3354,21 +3356,21 @@
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="16"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
-      <c r="V20" s="6"/>
-      <c r="W20" s="6"/>
-      <c r="X20" s="6"/>
-      <c r="Y20" s="6"/>
-      <c r="Z20" s="6"/>
-      <c r="AA20" s="6"/>
-      <c r="AB20" s="6"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="32"/>
+      <c r="R20" s="32"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="9"/>
+      <c r="AB20" s="9"/>
       <c r="AC20" s="6"/>
       <c r="AD20" s="6"/>
       <c r="AE20" s="6"/>
@@ -3454,18 +3456,18 @@
       <c r="DG20" s="6"/>
     </row>
     <row r="21" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>13</v>
+      <c r="A21" s="15" t="s">
+        <v>12</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
       <c r="D21" s="3">
         <v>5</v>
       </c>
-      <c r="E21" s="17" t="s">
-        <v>20</v>
+      <c r="E21" s="15" t="s">
+        <v>19</v>
       </c>
-      <c r="F21" s="19"/>
+      <c r="F21" s="17"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
@@ -3480,11 +3482,11 @@
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
       <c r="T21" s="6"/>
-      <c r="U21" s="12"/>
-      <c r="V21" s="12"/>
-      <c r="W21" s="12"/>
-      <c r="X21" s="12"/>
-      <c r="Y21" s="12"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="10"/>
       <c r="Z21" s="6"/>
       <c r="AA21" s="6"/>
       <c r="AB21" s="6"/>
@@ -3492,35 +3494,35 @@
       <c r="AD21" s="6"/>
       <c r="AE21" s="6"/>
       <c r="AF21" s="6"/>
-      <c r="AG21" s="6"/>
-      <c r="AH21" s="6"/>
-      <c r="AI21" s="6"/>
-      <c r="AJ21" s="6"/>
-      <c r="AK21" s="6"/>
-      <c r="AL21" s="6"/>
-      <c r="AM21" s="6"/>
-      <c r="AN21" s="6"/>
-      <c r="AO21" s="6"/>
-      <c r="AP21" s="6"/>
-      <c r="AQ21" s="6"/>
-      <c r="AR21" s="6"/>
-      <c r="AS21" s="6"/>
-      <c r="AT21" s="6"/>
-      <c r="AU21" s="6"/>
-      <c r="AV21" s="6"/>
-      <c r="AW21" s="6"/>
-      <c r="AX21" s="6"/>
-      <c r="AY21" s="6"/>
-      <c r="AZ21" s="6"/>
-      <c r="BA21" s="6"/>
-      <c r="BB21" s="6"/>
-      <c r="BC21" s="6"/>
-      <c r="BD21" s="6"/>
-      <c r="BE21" s="6"/>
-      <c r="BF21" s="6"/>
-      <c r="BG21" s="6"/>
-      <c r="BH21" s="6"/>
-      <c r="BI21" s="6"/>
+      <c r="AG21" s="9"/>
+      <c r="AH21" s="9"/>
+      <c r="AI21" s="9"/>
+      <c r="AJ21" s="9"/>
+      <c r="AK21" s="9"/>
+      <c r="AL21" s="9"/>
+      <c r="AM21" s="9"/>
+      <c r="AN21" s="9"/>
+      <c r="AO21" s="9"/>
+      <c r="AP21" s="9"/>
+      <c r="AQ21" s="9"/>
+      <c r="AR21" s="9"/>
+      <c r="AS21" s="9"/>
+      <c r="AT21" s="9"/>
+      <c r="AU21" s="9"/>
+      <c r="AV21" s="9"/>
+      <c r="AW21" s="9"/>
+      <c r="AX21" s="9"/>
+      <c r="AY21" s="9"/>
+      <c r="AZ21" s="9"/>
+      <c r="BA21" s="9"/>
+      <c r="BB21" s="9"/>
+      <c r="BC21" s="9"/>
+      <c r="BD21" s="9"/>
+      <c r="BE21" s="9"/>
+      <c r="BF21" s="9"/>
+      <c r="BG21" s="9"/>
+      <c r="BH21" s="9"/>
+      <c r="BI21" s="9"/>
       <c r="BJ21" s="6"/>
       <c r="BK21" s="6"/>
       <c r="BL21" s="6"/>
@@ -3573,18 +3575,18 @@
       <c r="DG21" s="6"/>
     </row>
     <row r="22" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
-        <v>14</v>
+      <c r="A22" s="15" t="s">
+        <v>13</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17"/>
       <c r="D22" s="3">
         <v>5</v>
       </c>
-      <c r="E22" s="17" t="s">
-        <v>23</v>
+      <c r="E22" s="15" t="s">
+        <v>22</v>
       </c>
-      <c r="F22" s="19"/>
+      <c r="F22" s="17"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
@@ -3599,11 +3601,11 @@
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
       <c r="T22" s="6"/>
-      <c r="U22" s="12"/>
-      <c r="V22" s="12"/>
-      <c r="W22" s="12"/>
-      <c r="X22" s="12"/>
-      <c r="Y22" s="12"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="10"/>
       <c r="Z22" s="6"/>
       <c r="AA22" s="6"/>
       <c r="AB22" s="6"/>
@@ -3611,36 +3613,36 @@
       <c r="AD22" s="6"/>
       <c r="AE22" s="6"/>
       <c r="AF22" s="6"/>
-      <c r="AG22" s="6"/>
-      <c r="AH22" s="6"/>
-      <c r="AI22" s="6"/>
-      <c r="AJ22" s="6"/>
-      <c r="AK22" s="6"/>
-      <c r="AL22" s="6"/>
-      <c r="AM22" s="6"/>
-      <c r="AN22" s="6"/>
-      <c r="AO22" s="6"/>
-      <c r="AP22" s="6"/>
-      <c r="AQ22" s="6"/>
-      <c r="AR22" s="6"/>
-      <c r="AS22" s="6"/>
-      <c r="AT22" s="6"/>
-      <c r="AU22" s="6"/>
-      <c r="AV22" s="6"/>
-      <c r="AW22" s="6"/>
-      <c r="AX22" s="6"/>
-      <c r="AY22" s="6"/>
-      <c r="AZ22" s="6"/>
-      <c r="BA22" s="6"/>
-      <c r="BB22" s="6"/>
-      <c r="BC22" s="6"/>
-      <c r="BD22" s="6"/>
-      <c r="BE22" s="6"/>
-      <c r="BF22" s="6"/>
-      <c r="BG22" s="6"/>
-      <c r="BH22" s="6"/>
-      <c r="BI22" s="6"/>
-      <c r="BJ22" s="6"/>
+      <c r="AG22" s="9"/>
+      <c r="AH22" s="9"/>
+      <c r="AI22" s="9"/>
+      <c r="AJ22" s="9"/>
+      <c r="AK22" s="9"/>
+      <c r="AL22" s="9"/>
+      <c r="AM22" s="9"/>
+      <c r="AN22" s="9"/>
+      <c r="AO22" s="9"/>
+      <c r="AP22" s="9"/>
+      <c r="AQ22" s="9"/>
+      <c r="AR22" s="9"/>
+      <c r="AS22" s="9"/>
+      <c r="AT22" s="9"/>
+      <c r="AU22" s="9"/>
+      <c r="AV22" s="9"/>
+      <c r="AW22" s="9"/>
+      <c r="AX22" s="9"/>
+      <c r="AY22" s="9"/>
+      <c r="AZ22" s="9"/>
+      <c r="BA22" s="9"/>
+      <c r="BB22" s="9"/>
+      <c r="BC22" s="9"/>
+      <c r="BD22" s="9"/>
+      <c r="BE22" s="9"/>
+      <c r="BF22" s="9"/>
+      <c r="BG22" s="9"/>
+      <c r="BH22" s="9"/>
+      <c r="BI22" s="9"/>
+      <c r="BJ22" s="9"/>
       <c r="BK22" s="6"/>
       <c r="BL22" s="6"/>
       <c r="BM22" s="6"/>
@@ -3692,18 +3694,18 @@
       <c r="DG22" s="6"/>
     </row>
     <row r="23" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
-        <v>15</v>
+      <c r="A23" s="15" t="s">
+        <v>14</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="17"/>
       <c r="D23" s="3">
         <v>5</v>
       </c>
-      <c r="E23" s="17" t="s">
-        <v>23</v>
+      <c r="E23" s="15" t="s">
+        <v>22</v>
       </c>
-      <c r="F23" s="19"/>
+      <c r="F23" s="17"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
@@ -3718,11 +3720,11 @@
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
       <c r="T23" s="6"/>
-      <c r="U23" s="12"/>
-      <c r="V23" s="12"/>
-      <c r="W23" s="12"/>
-      <c r="X23" s="12"/>
-      <c r="Y23" s="12"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="10"/>
+      <c r="Y23" s="10"/>
       <c r="Z23" s="6"/>
       <c r="AA23" s="6"/>
       <c r="AB23" s="6"/>
@@ -3730,41 +3732,41 @@
       <c r="AD23" s="6"/>
       <c r="AE23" s="6"/>
       <c r="AF23" s="6"/>
-      <c r="AG23" s="6"/>
-      <c r="AH23" s="6"/>
-      <c r="AI23" s="6"/>
-      <c r="AJ23" s="6"/>
-      <c r="AK23" s="6"/>
-      <c r="AL23" s="6"/>
-      <c r="AM23" s="6"/>
-      <c r="AN23" s="6"/>
-      <c r="AO23" s="6"/>
-      <c r="AP23" s="6"/>
-      <c r="AQ23" s="6"/>
-      <c r="AR23" s="6"/>
-      <c r="AS23" s="6"/>
-      <c r="AT23" s="6"/>
-      <c r="AU23" s="6"/>
-      <c r="AV23" s="6"/>
-      <c r="AW23" s="6"/>
-      <c r="AX23" s="6"/>
-      <c r="AY23" s="6"/>
-      <c r="AZ23" s="6"/>
-      <c r="BA23" s="6"/>
-      <c r="BB23" s="6"/>
-      <c r="BC23" s="6"/>
-      <c r="BD23" s="6"/>
-      <c r="BE23" s="6"/>
-      <c r="BF23" s="6"/>
-      <c r="BG23" s="6"/>
-      <c r="BH23" s="6"/>
-      <c r="BI23" s="6"/>
-      <c r="BJ23" s="6"/>
-      <c r="BK23" s="6"/>
-      <c r="BL23" s="6"/>
-      <c r="BM23" s="6"/>
-      <c r="BN23" s="6"/>
-      <c r="BO23" s="6"/>
+      <c r="AG23" s="9"/>
+      <c r="AH23" s="9"/>
+      <c r="AI23" s="9"/>
+      <c r="AJ23" s="9"/>
+      <c r="AK23" s="9"/>
+      <c r="AL23" s="9"/>
+      <c r="AM23" s="9"/>
+      <c r="AN23" s="9"/>
+      <c r="AO23" s="9"/>
+      <c r="AP23" s="9"/>
+      <c r="AQ23" s="9"/>
+      <c r="AR23" s="9"/>
+      <c r="AS23" s="9"/>
+      <c r="AT23" s="9"/>
+      <c r="AU23" s="9"/>
+      <c r="AV23" s="9"/>
+      <c r="AW23" s="9"/>
+      <c r="AX23" s="9"/>
+      <c r="AY23" s="9"/>
+      <c r="AZ23" s="9"/>
+      <c r="BA23" s="9"/>
+      <c r="BB23" s="9"/>
+      <c r="BC23" s="9"/>
+      <c r="BD23" s="9"/>
+      <c r="BE23" s="9"/>
+      <c r="BF23" s="9"/>
+      <c r="BG23" s="9"/>
+      <c r="BH23" s="9"/>
+      <c r="BI23" s="9"/>
+      <c r="BJ23" s="9"/>
+      <c r="BK23" s="9"/>
+      <c r="BL23" s="9"/>
+      <c r="BM23" s="9"/>
+      <c r="BN23" s="9"/>
+      <c r="BO23" s="9"/>
       <c r="BP23" s="6"/>
       <c r="BQ23" s="6"/>
       <c r="BR23" s="6"/>
@@ -3811,18 +3813,18 @@
       <c r="DG23" s="6"/>
     </row>
     <row r="24" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
-        <v>16</v>
+      <c r="A24" s="22" t="s">
+        <v>15</v>
       </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="27"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="4">
         <v>5</v>
       </c>
-      <c r="E24" s="26" t="s">
-        <v>21</v>
+      <c r="E24" s="22" t="s">
+        <v>20</v>
       </c>
-      <c r="F24" s="27"/>
+      <c r="F24" s="24"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
@@ -3844,11 +3846,11 @@
       <c r="Y24" s="6"/>
       <c r="Z24" s="6"/>
       <c r="AA24" s="6"/>
-      <c r="AB24" s="12"/>
-      <c r="AC24" s="12"/>
-      <c r="AD24" s="12"/>
-      <c r="AE24" s="12"/>
-      <c r="AF24" s="12"/>
+      <c r="AB24" s="10"/>
+      <c r="AC24" s="10"/>
+      <c r="AD24" s="10"/>
+      <c r="AE24" s="10"/>
+      <c r="AF24" s="10"/>
       <c r="AG24" s="6"/>
       <c r="AH24" s="6"/>
       <c r="AI24" s="6"/>
@@ -3859,33 +3861,33 @@
       <c r="AN24" s="6"/>
       <c r="AO24" s="6"/>
       <c r="AP24" s="6"/>
-      <c r="AQ24" s="6"/>
-      <c r="AR24" s="6"/>
-      <c r="AS24" s="6"/>
-      <c r="AT24" s="6"/>
-      <c r="AU24" s="6"/>
-      <c r="AV24" s="6"/>
-      <c r="AW24" s="6"/>
-      <c r="AX24" s="6"/>
-      <c r="AY24" s="6"/>
-      <c r="AZ24" s="6"/>
-      <c r="BA24" s="6"/>
-      <c r="BB24" s="6"/>
-      <c r="BC24" s="6"/>
-      <c r="BD24" s="6"/>
-      <c r="BE24" s="6"/>
-      <c r="BF24" s="6"/>
-      <c r="BG24" s="6"/>
-      <c r="BH24" s="6"/>
-      <c r="BI24" s="6"/>
-      <c r="BJ24" s="6"/>
-      <c r="BK24" s="6"/>
-      <c r="BL24" s="6"/>
-      <c r="BM24" s="6"/>
-      <c r="BN24" s="6"/>
-      <c r="BO24" s="6"/>
-      <c r="BP24" s="6"/>
-      <c r="BQ24" s="6"/>
+      <c r="AQ24" s="9"/>
+      <c r="AR24" s="9"/>
+      <c r="AS24" s="9"/>
+      <c r="AT24" s="9"/>
+      <c r="AU24" s="9"/>
+      <c r="AV24" s="9"/>
+      <c r="AW24" s="9"/>
+      <c r="AX24" s="9"/>
+      <c r="AY24" s="9"/>
+      <c r="AZ24" s="9"/>
+      <c r="BA24" s="9"/>
+      <c r="BB24" s="9"/>
+      <c r="BC24" s="9"/>
+      <c r="BD24" s="9"/>
+      <c r="BE24" s="9"/>
+      <c r="BF24" s="9"/>
+      <c r="BG24" s="9"/>
+      <c r="BH24" s="9"/>
+      <c r="BI24" s="9"/>
+      <c r="BJ24" s="9"/>
+      <c r="BK24" s="9"/>
+      <c r="BL24" s="9"/>
+      <c r="BM24" s="9"/>
+      <c r="BN24" s="9"/>
+      <c r="BO24" s="9"/>
+      <c r="BP24" s="9"/>
+      <c r="BQ24" s="9"/>
       <c r="BR24" s="6"/>
       <c r="BS24" s="6"/>
       <c r="BT24" s="6"/>
@@ -3930,18 +3932,18 @@
       <c r="DG24" s="6"/>
     </row>
     <row r="25" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
-        <v>17</v>
+      <c r="A25" s="15" t="s">
+        <v>16</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="17"/>
       <c r="D25" s="3">
         <v>5</v>
       </c>
-      <c r="E25" s="17" t="s">
-        <v>22</v>
+      <c r="E25" s="15" t="s">
+        <v>21</v>
       </c>
-      <c r="F25" s="19"/>
+      <c r="F25" s="17"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
@@ -3966,11 +3968,11 @@
       <c r="AB25" s="6"/>
       <c r="AC25" s="6"/>
       <c r="AD25" s="6"/>
-      <c r="AE25" s="12"/>
-      <c r="AF25" s="12"/>
-      <c r="AG25" s="12"/>
-      <c r="AH25" s="12"/>
-      <c r="AI25" s="12"/>
+      <c r="AE25" s="10"/>
+      <c r="AF25" s="10"/>
+      <c r="AG25" s="10"/>
+      <c r="AH25" s="10"/>
+      <c r="AI25" s="10"/>
       <c r="AJ25" s="6"/>
       <c r="AK25" s="6"/>
       <c r="AL25" s="6"/>
@@ -3992,23 +3994,23 @@
       <c r="BB25" s="6"/>
       <c r="BC25" s="6"/>
       <c r="BD25" s="6"/>
-      <c r="BE25" s="6"/>
-      <c r="BF25" s="6"/>
-      <c r="BG25" s="6"/>
-      <c r="BH25" s="6"/>
-      <c r="BI25" s="6"/>
-      <c r="BJ25" s="6"/>
-      <c r="BK25" s="6"/>
-      <c r="BL25" s="6"/>
-      <c r="BM25" s="6"/>
-      <c r="BN25" s="6"/>
-      <c r="BO25" s="6"/>
-      <c r="BP25" s="6"/>
-      <c r="BQ25" s="6"/>
-      <c r="BR25" s="6"/>
-      <c r="BS25" s="6"/>
-      <c r="BT25" s="6"/>
-      <c r="BU25" s="6"/>
+      <c r="BE25" s="9"/>
+      <c r="BF25" s="9"/>
+      <c r="BG25" s="9"/>
+      <c r="BH25" s="9"/>
+      <c r="BI25" s="9"/>
+      <c r="BJ25" s="9"/>
+      <c r="BK25" s="9"/>
+      <c r="BL25" s="9"/>
+      <c r="BM25" s="9"/>
+      <c r="BN25" s="9"/>
+      <c r="BO25" s="9"/>
+      <c r="BP25" s="9"/>
+      <c r="BQ25" s="9"/>
+      <c r="BR25" s="9"/>
+      <c r="BS25" s="9"/>
+      <c r="BT25" s="9"/>
+      <c r="BU25" s="9"/>
       <c r="BV25" s="6"/>
       <c r="BW25" s="6"/>
       <c r="BX25" s="6"/>
@@ -4049,18 +4051,18 @@
       <c r="DG25" s="6"/>
     </row>
     <row r="26" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
-        <v>18</v>
+      <c r="A26" s="15" t="s">
+        <v>17</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
       <c r="D26" s="3">
         <v>8</v>
       </c>
-      <c r="E26" s="17" t="s">
-        <v>22</v>
+      <c r="E26" s="15" t="s">
+        <v>21</v>
       </c>
-      <c r="F26" s="19"/>
+      <c r="F26" s="17"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
@@ -4089,46 +4091,46 @@
       <c r="AF26" s="6"/>
       <c r="AG26" s="6"/>
       <c r="AH26" s="6"/>
-      <c r="AI26" s="12"/>
-      <c r="AJ26" s="12"/>
-      <c r="AK26" s="12"/>
-      <c r="AL26" s="12"/>
-      <c r="AM26" s="12"/>
-      <c r="AN26" s="12"/>
-      <c r="AO26" s="12"/>
-      <c r="AP26" s="12"/>
-      <c r="AQ26" s="6"/>
-      <c r="AR26" s="6"/>
-      <c r="AS26" s="6"/>
-      <c r="AT26" s="6"/>
-      <c r="AU26" s="6"/>
-      <c r="AV26" s="6"/>
-      <c r="AW26" s="6"/>
-      <c r="AX26" s="6"/>
-      <c r="AY26" s="6"/>
-      <c r="AZ26" s="6"/>
-      <c r="BA26" s="6"/>
-      <c r="BB26" s="6"/>
-      <c r="BC26" s="6"/>
-      <c r="BD26" s="6"/>
-      <c r="BE26" s="6"/>
-      <c r="BF26" s="6"/>
-      <c r="BG26" s="6"/>
-      <c r="BH26" s="6"/>
-      <c r="BI26" s="6"/>
-      <c r="BJ26" s="6"/>
-      <c r="BK26" s="6"/>
-      <c r="BL26" s="6"/>
-      <c r="BM26" s="6"/>
-      <c r="BN26" s="6"/>
-      <c r="BO26" s="6"/>
-      <c r="BP26" s="6"/>
-      <c r="BQ26" s="6"/>
-      <c r="BR26" s="6"/>
-      <c r="BS26" s="6"/>
-      <c r="BT26" s="6"/>
-      <c r="BU26" s="6"/>
-      <c r="BV26" s="6"/>
+      <c r="AI26" s="10"/>
+      <c r="AJ26" s="10"/>
+      <c r="AK26" s="10"/>
+      <c r="AL26" s="10"/>
+      <c r="AM26" s="10"/>
+      <c r="AN26" s="10"/>
+      <c r="AO26" s="10"/>
+      <c r="AP26" s="10"/>
+      <c r="AQ26" s="10"/>
+      <c r="AR26" s="10"/>
+      <c r="AS26" s="10"/>
+      <c r="AT26" s="10"/>
+      <c r="AU26" s="10"/>
+      <c r="AV26" s="10"/>
+      <c r="AW26" s="10"/>
+      <c r="AX26" s="10"/>
+      <c r="AY26" s="10"/>
+      <c r="AZ26" s="10"/>
+      <c r="BA26" s="10"/>
+      <c r="BB26" s="10"/>
+      <c r="BC26" s="10"/>
+      <c r="BD26" s="10"/>
+      <c r="BE26" s="10"/>
+      <c r="BF26" s="10"/>
+      <c r="BG26" s="32"/>
+      <c r="BH26" s="32"/>
+      <c r="BI26" s="32"/>
+      <c r="BJ26" s="32"/>
+      <c r="BK26" s="32"/>
+      <c r="BL26" s="32"/>
+      <c r="BM26" s="32"/>
+      <c r="BN26" s="32"/>
+      <c r="BO26" s="32"/>
+      <c r="BP26" s="32"/>
+      <c r="BQ26" s="32"/>
+      <c r="BR26" s="32"/>
+      <c r="BS26" s="32"/>
+      <c r="BT26" s="32"/>
+      <c r="BU26" s="32"/>
+      <c r="BV26" s="32"/>
       <c r="BW26" s="6"/>
       <c r="BX26" s="6"/>
       <c r="BY26" s="6"/>
@@ -4168,9 +4170,9 @@
       <c r="DG26" s="6"/>
     </row>
     <row r="27" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
@@ -4281,11 +4283,9 @@
       <c r="DG27" s="6"/>
     </row>
     <row r="28" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="25"/>
+      <c r="A28" s="33"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -4396,89 +4396,89 @@
       <c r="DG28" s="6"/>
     </row>
     <row r="29" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
-        <v>25</v>
+      <c r="A29" s="42" t="s">
+        <v>31</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="3">
-        <v>2</v>
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="41">
+        <v>5</v>
       </c>
-      <c r="E29" s="21" t="s">
-        <v>21</v>
+      <c r="E29" s="40" t="s">
+        <v>23</v>
       </c>
-      <c r="F29" s="22"/>
+      <c r="F29" s="40"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
-      <c r="S29" s="6"/>
-      <c r="T29" s="6"/>
-      <c r="U29" s="6"/>
-      <c r="V29" s="6"/>
-      <c r="W29" s="6"/>
-      <c r="X29" s="6"/>
-      <c r="Y29" s="6"/>
-      <c r="Z29" s="6"/>
-      <c r="AA29" s="6"/>
-      <c r="AB29" s="6"/>
-      <c r="AC29" s="6"/>
-      <c r="AD29" s="6"/>
-      <c r="AE29" s="6"/>
-      <c r="AF29" s="6"/>
-      <c r="AG29" s="6"/>
-      <c r="AH29" s="6"/>
-      <c r="AI29" s="12"/>
-      <c r="AJ29" s="12"/>
-      <c r="AK29" s="6"/>
-      <c r="AL29" s="6"/>
-      <c r="AM29" s="6"/>
-      <c r="AN29" s="6"/>
-      <c r="AO29" s="6"/>
-      <c r="AP29" s="6"/>
-      <c r="AQ29" s="6"/>
-      <c r="AR29" s="6"/>
-      <c r="AS29" s="6"/>
-      <c r="AT29" s="6"/>
-      <c r="AU29" s="6"/>
-      <c r="AV29" s="6"/>
-      <c r="AW29" s="6"/>
-      <c r="AX29" s="6"/>
-      <c r="AY29" s="6"/>
-      <c r="AZ29" s="6"/>
-      <c r="BA29" s="6"/>
-      <c r="BB29" s="6"/>
-      <c r="BC29" s="6"/>
-      <c r="BD29" s="6"/>
-      <c r="BE29" s="6"/>
-      <c r="BF29" s="6"/>
-      <c r="BG29" s="6"/>
-      <c r="BH29" s="6"/>
-      <c r="BI29" s="6"/>
-      <c r="BJ29" s="6"/>
-      <c r="BK29" s="6"/>
-      <c r="BL29" s="6"/>
-      <c r="BM29" s="6"/>
-      <c r="BN29" s="6"/>
-      <c r="BO29" s="6"/>
-      <c r="BP29" s="6"/>
-      <c r="BQ29" s="6"/>
-      <c r="BR29" s="6"/>
-      <c r="BS29" s="6"/>
-      <c r="BT29" s="6"/>
-      <c r="BU29" s="6"/>
-      <c r="BV29" s="6"/>
-      <c r="BW29" s="6"/>
-      <c r="BX29" s="6"/>
-      <c r="BY29" s="6"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="9"/>
+      <c r="V29" s="9"/>
+      <c r="W29" s="9"/>
+      <c r="X29" s="9"/>
+      <c r="Y29" s="9"/>
+      <c r="Z29" s="9"/>
+      <c r="AA29" s="9"/>
+      <c r="AB29" s="9"/>
+      <c r="AC29" s="9"/>
+      <c r="AD29" s="9"/>
+      <c r="AE29" s="9"/>
+      <c r="AF29" s="9"/>
+      <c r="AG29" s="9"/>
+      <c r="AH29" s="9"/>
+      <c r="AI29" s="43"/>
+      <c r="AJ29" s="43"/>
+      <c r="AK29" s="9"/>
+      <c r="AL29" s="9"/>
+      <c r="AM29" s="9"/>
+      <c r="AN29" s="9"/>
+      <c r="AO29" s="9"/>
+      <c r="AP29" s="9"/>
+      <c r="AQ29" s="9"/>
+      <c r="AR29" s="9"/>
+      <c r="AS29" s="9"/>
+      <c r="AT29" s="9"/>
+      <c r="AU29" s="9"/>
+      <c r="AV29" s="9"/>
+      <c r="AW29" s="9"/>
+      <c r="AX29" s="9"/>
+      <c r="AY29" s="9"/>
+      <c r="AZ29" s="9"/>
+      <c r="BA29" s="9"/>
+      <c r="BB29" s="9"/>
+      <c r="BC29" s="9"/>
+      <c r="BD29" s="9"/>
+      <c r="BE29" s="9"/>
+      <c r="BF29" s="9"/>
+      <c r="BG29" s="9"/>
+      <c r="BH29" s="9"/>
+      <c r="BI29" s="9"/>
+      <c r="BJ29" s="9"/>
+      <c r="BK29" s="9"/>
+      <c r="BL29" s="9"/>
+      <c r="BM29" s="9"/>
+      <c r="BN29" s="9"/>
+      <c r="BO29" s="9"/>
+      <c r="BP29" s="9"/>
+      <c r="BQ29" s="9"/>
+      <c r="BR29" s="9"/>
+      <c r="BS29" s="9"/>
+      <c r="BT29" s="9"/>
+      <c r="BU29" s="9"/>
+      <c r="BV29" s="9"/>
+      <c r="BW29" s="9"/>
+      <c r="BX29" s="9"/>
+      <c r="BY29" s="9"/>
       <c r="BZ29" s="6"/>
       <c r="CA29" s="6"/>
       <c r="CB29" s="6"/>
@@ -4515,18 +4515,12 @@
       <c r="DG29" s="6"/>
     </row>
     <row r="30" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="3">
-        <v>10</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F30" s="19"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
@@ -4558,16 +4552,16 @@
       <c r="AI30" s="6"/>
       <c r="AJ30" s="6"/>
       <c r="AK30" s="6"/>
-      <c r="AL30" s="12"/>
-      <c r="AM30" s="12"/>
-      <c r="AN30" s="12"/>
-      <c r="AO30" s="12"/>
-      <c r="AP30" s="12"/>
-      <c r="AQ30" s="12"/>
-      <c r="AR30" s="12"/>
-      <c r="AS30" s="12"/>
-      <c r="AT30" s="12"/>
-      <c r="AU30" s="12"/>
+      <c r="AL30" s="33"/>
+      <c r="AM30" s="33"/>
+      <c r="AN30" s="33"/>
+      <c r="AO30" s="33"/>
+      <c r="AP30" s="33"/>
+      <c r="AQ30" s="33"/>
+      <c r="AR30" s="33"/>
+      <c r="AS30" s="33"/>
+      <c r="AT30" s="33"/>
+      <c r="AU30" s="33"/>
       <c r="AV30" s="6"/>
       <c r="AW30" s="6"/>
       <c r="AX30" s="6"/>
@@ -4634,18 +4628,12 @@
       <c r="DG30" s="6"/>
     </row>
     <row r="31" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="3">
-        <v>15</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F31" s="19"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
@@ -4677,21 +4665,21 @@
       <c r="AI31" s="6"/>
       <c r="AJ31" s="6"/>
       <c r="AK31" s="6"/>
-      <c r="AL31" s="12"/>
-      <c r="AM31" s="12"/>
-      <c r="AN31" s="12"/>
-      <c r="AO31" s="12"/>
-      <c r="AP31" s="12"/>
-      <c r="AQ31" s="12"/>
-      <c r="AR31" s="12"/>
-      <c r="AS31" s="12"/>
-      <c r="AT31" s="12"/>
-      <c r="AU31" s="12"/>
-      <c r="AV31" s="12"/>
-      <c r="AW31" s="12"/>
-      <c r="AX31" s="12"/>
-      <c r="AY31" s="12"/>
-      <c r="AZ31" s="12"/>
+      <c r="AL31" s="33"/>
+      <c r="AM31" s="33"/>
+      <c r="AN31" s="33"/>
+      <c r="AO31" s="33"/>
+      <c r="AP31" s="33"/>
+      <c r="AQ31" s="33"/>
+      <c r="AR31" s="33"/>
+      <c r="AS31" s="33"/>
+      <c r="AT31" s="33"/>
+      <c r="AU31" s="33"/>
+      <c r="AV31" s="33"/>
+      <c r="AW31" s="33"/>
+      <c r="AX31" s="33"/>
+      <c r="AY31" s="33"/>
+      <c r="AZ31" s="33"/>
       <c r="BA31" s="6"/>
       <c r="BB31" s="6"/>
       <c r="BC31" s="6"/>
@@ -4753,18 +4741,12 @@
       <c r="DG31" s="6"/>
     </row>
     <row r="32" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="3">
-        <v>20</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F32" s="19"/>
+      <c r="A32" s="33"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
@@ -4814,26 +4796,26 @@
       <c r="BA32" s="6"/>
       <c r="BB32" s="6"/>
       <c r="BC32" s="6"/>
-      <c r="BD32" s="12"/>
-      <c r="BE32" s="12"/>
-      <c r="BF32" s="12"/>
-      <c r="BG32" s="12"/>
-      <c r="BH32" s="12"/>
-      <c r="BI32" s="12"/>
-      <c r="BJ32" s="12"/>
-      <c r="BK32" s="12"/>
-      <c r="BL32" s="12"/>
-      <c r="BM32" s="12"/>
-      <c r="BN32" s="12"/>
-      <c r="BO32" s="12"/>
-      <c r="BP32" s="12"/>
-      <c r="BQ32" s="12"/>
-      <c r="BR32" s="12"/>
-      <c r="BS32" s="12"/>
-      <c r="BT32" s="12"/>
-      <c r="BU32" s="12"/>
-      <c r="BV32" s="12"/>
-      <c r="BW32" s="12"/>
+      <c r="BD32" s="10"/>
+      <c r="BE32" s="10"/>
+      <c r="BF32" s="10"/>
+      <c r="BG32" s="10"/>
+      <c r="BH32" s="10"/>
+      <c r="BI32" s="10"/>
+      <c r="BJ32" s="10"/>
+      <c r="BK32" s="10"/>
+      <c r="BL32" s="10"/>
+      <c r="BM32" s="10"/>
+      <c r="BN32" s="10"/>
+      <c r="BO32" s="10"/>
+      <c r="BP32" s="10"/>
+      <c r="BQ32" s="10"/>
+      <c r="BR32" s="10"/>
+      <c r="BS32" s="10"/>
+      <c r="BT32" s="10"/>
+      <c r="BU32" s="10"/>
+      <c r="BV32" s="10"/>
+      <c r="BW32" s="10"/>
       <c r="BX32" s="6"/>
       <c r="BY32" s="6"/>
       <c r="BZ32" s="6"/>
@@ -4872,18 +4854,12 @@
       <c r="DG32" s="6"/>
     </row>
     <row r="33" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="3">
-        <v>10</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F33" s="19"/>
+      <c r="A33" s="33"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -4929,16 +4905,16 @@
       <c r="AW33" s="6"/>
       <c r="AX33" s="6"/>
       <c r="AY33" s="6"/>
-      <c r="AZ33" s="12"/>
-      <c r="BA33" s="12"/>
-      <c r="BB33" s="12"/>
-      <c r="BC33" s="12"/>
-      <c r="BD33" s="12"/>
-      <c r="BE33" s="12"/>
-      <c r="BF33" s="12"/>
-      <c r="BG33" s="12"/>
-      <c r="BH33" s="12"/>
-      <c r="BI33" s="12"/>
+      <c r="AZ33" s="33"/>
+      <c r="BA33" s="33"/>
+      <c r="BB33" s="33"/>
+      <c r="BC33" s="33"/>
+      <c r="BD33" s="33"/>
+      <c r="BE33" s="33"/>
+      <c r="BF33" s="33"/>
+      <c r="BG33" s="33"/>
+      <c r="BH33" s="33"/>
+      <c r="BI33" s="33"/>
       <c r="BJ33" s="6"/>
       <c r="BK33" s="6"/>
       <c r="BL33" s="6"/>
@@ -4991,9 +4967,9 @@
       <c r="DG33" s="6"/>
     </row>
     <row r="34" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -5104,11 +5080,9 @@
       <c r="DG34" s="6"/>
     </row>
     <row r="35" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A35" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35" s="24"/>
-      <c r="C35" s="25"/>
+      <c r="A35" s="33"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
@@ -5219,18 +5193,12 @@
       <c r="DG35" s="6"/>
     </row>
     <row r="36" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="3">
-        <v>5</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F36" s="19"/>
+      <c r="A36" s="33"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -5299,11 +5267,11 @@
       <c r="BT36" s="6"/>
       <c r="BU36" s="6"/>
       <c r="BV36" s="6"/>
-      <c r="BW36" s="14"/>
-      <c r="BX36" s="14"/>
-      <c r="BY36" s="14"/>
-      <c r="BZ36" s="14"/>
-      <c r="CA36" s="14"/>
+      <c r="BW36" s="39"/>
+      <c r="BX36" s="39"/>
+      <c r="BY36" s="39"/>
+      <c r="BZ36" s="39"/>
+      <c r="CA36" s="39"/>
       <c r="CB36" s="6"/>
       <c r="CC36" s="6"/>
       <c r="CD36" s="6"/>
@@ -5338,18 +5306,12 @@
       <c r="DG36" s="6"/>
     </row>
     <row r="37" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A37" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="3">
-        <v>5</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F37" s="19"/>
+      <c r="A37" s="33"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="33"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -5418,11 +5380,11 @@
       <c r="BT37" s="6"/>
       <c r="BU37" s="6"/>
       <c r="BV37" s="6"/>
-      <c r="BW37" s="12"/>
-      <c r="BX37" s="12"/>
-      <c r="BY37" s="12"/>
-      <c r="BZ37" s="12"/>
-      <c r="CA37" s="12"/>
+      <c r="BW37" s="10"/>
+      <c r="BX37" s="10"/>
+      <c r="BY37" s="10"/>
+      <c r="BZ37" s="10"/>
+      <c r="CA37" s="10"/>
       <c r="CB37" s="6"/>
       <c r="CC37" s="6"/>
       <c r="CD37" s="6"/>
@@ -5457,18 +5419,12 @@
       <c r="DG37" s="6"/>
     </row>
     <row r="38" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="3">
-        <v>5</v>
-      </c>
-      <c r="E38" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F38" s="19"/>
+      <c r="A38" s="33"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="33"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -5537,11 +5493,11 @@
       <c r="BT38" s="6"/>
       <c r="BU38" s="6"/>
       <c r="BV38" s="6"/>
-      <c r="BW38" s="12"/>
-      <c r="BX38" s="12"/>
-      <c r="BY38" s="12"/>
-      <c r="BZ38" s="12"/>
-      <c r="CA38" s="12"/>
+      <c r="BW38" s="10"/>
+      <c r="BX38" s="10"/>
+      <c r="BY38" s="10"/>
+      <c r="BZ38" s="10"/>
+      <c r="CA38" s="10"/>
       <c r="CB38" s="6"/>
       <c r="CC38" s="6"/>
       <c r="CD38" s="6"/>
@@ -5576,18 +5532,12 @@
       <c r="DG38" s="6"/>
     </row>
     <row r="39" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="3">
-        <v>5</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F39" s="19"/>
+      <c r="A39" s="33"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -5656,11 +5606,11 @@
       <c r="BT39" s="6"/>
       <c r="BU39" s="6"/>
       <c r="BV39" s="6"/>
-      <c r="BW39" s="12"/>
-      <c r="BX39" s="12"/>
-      <c r="BY39" s="12"/>
-      <c r="BZ39" s="12"/>
-      <c r="CA39" s="12"/>
+      <c r="BW39" s="10"/>
+      <c r="BX39" s="10"/>
+      <c r="BY39" s="10"/>
+      <c r="BZ39" s="10"/>
+      <c r="CA39" s="10"/>
       <c r="CB39" s="6"/>
       <c r="CC39" s="6"/>
       <c r="CD39" s="6"/>
@@ -5695,18 +5645,12 @@
       <c r="DG39" s="6"/>
     </row>
     <row r="40" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="3">
-        <v>5</v>
-      </c>
-      <c r="E40" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F40" s="19"/>
+      <c r="A40" s="33"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
@@ -5775,11 +5719,11 @@
       <c r="BT40" s="6"/>
       <c r="BU40" s="6"/>
       <c r="BV40" s="6"/>
-      <c r="BW40" s="12"/>
-      <c r="BX40" s="12"/>
-      <c r="BY40" s="12"/>
-      <c r="BZ40" s="12"/>
-      <c r="CA40" s="12"/>
+      <c r="BW40" s="10"/>
+      <c r="BX40" s="10"/>
+      <c r="BY40" s="10"/>
+      <c r="BZ40" s="10"/>
+      <c r="CA40" s="10"/>
       <c r="CB40" s="6"/>
       <c r="CC40" s="6"/>
       <c r="CD40" s="6"/>
@@ -5814,18 +5758,12 @@
       <c r="DG40" s="6"/>
     </row>
     <row r="41" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A41" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="3">
-        <v>5</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F41" s="19"/>
+      <c r="A41" s="33"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
@@ -5894,11 +5832,11 @@
       <c r="BT41" s="6"/>
       <c r="BU41" s="6"/>
       <c r="BV41" s="6"/>
-      <c r="BW41" s="12"/>
-      <c r="BX41" s="12"/>
-      <c r="BY41" s="12"/>
-      <c r="BZ41" s="12"/>
-      <c r="CA41" s="12"/>
+      <c r="BW41" s="10"/>
+      <c r="BX41" s="10"/>
+      <c r="BY41" s="10"/>
+      <c r="BZ41" s="10"/>
+      <c r="CA41" s="10"/>
       <c r="CB41" s="6"/>
       <c r="CC41" s="6"/>
       <c r="CD41" s="6"/>
@@ -5933,18 +5871,12 @@
       <c r="DG41" s="6"/>
     </row>
     <row r="42" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="3">
-        <v>5</v>
-      </c>
-      <c r="E42" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F42" s="19"/>
+      <c r="A42" s="33"/>
+      <c r="B42" s="33"/>
+      <c r="C42" s="33"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="33"/>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
@@ -6013,11 +5945,11 @@
       <c r="BT42" s="6"/>
       <c r="BU42" s="6"/>
       <c r="BV42" s="6"/>
-      <c r="BW42" s="13"/>
-      <c r="BX42" s="13"/>
-      <c r="BY42" s="13"/>
-      <c r="BZ42" s="13"/>
-      <c r="CA42" s="13"/>
+      <c r="BW42" s="18"/>
+      <c r="BX42" s="18"/>
+      <c r="BY42" s="18"/>
+      <c r="BZ42" s="18"/>
+      <c r="CA42" s="18"/>
       <c r="CB42" s="6"/>
       <c r="CC42" s="6"/>
       <c r="CD42" s="6"/>
@@ -6052,9 +5984,9 @@
       <c r="DG42" s="6"/>
     </row>
     <row r="43" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
@@ -6165,11 +6097,9 @@
       <c r="DG43" s="6"/>
     </row>
     <row r="44" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A44" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B44" s="24"/>
-      <c r="C44" s="25"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="33"/>
+      <c r="C44" s="33"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
@@ -6280,18 +6210,12 @@
       <c r="DG44" s="6"/>
     </row>
     <row r="45" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A45" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="3">
-        <v>1</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F45" s="19"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
@@ -6365,7 +6289,7 @@
       <c r="BY45" s="6"/>
       <c r="BZ45" s="6"/>
       <c r="CA45" s="6"/>
-      <c r="CB45" s="11"/>
+      <c r="CB45" s="6"/>
       <c r="CC45" s="6"/>
       <c r="CD45" s="6"/>
       <c r="CE45" s="6"/>
@@ -6399,9 +6323,9 @@
       <c r="DG45" s="6"/>
     </row>
     <row r="46" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A46" s="20"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
@@ -6512,89 +6436,85 @@
       <c r="DG46" s="6"/>
     </row>
     <row r="47" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A47" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="19"/>
-      <c r="E47" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="F47" s="19"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="9"/>
-      <c r="L47" s="9"/>
-      <c r="M47" s="9"/>
-      <c r="N47" s="9"/>
-      <c r="O47" s="9"/>
-      <c r="P47" s="9"/>
-      <c r="Q47" s="9"/>
-      <c r="R47" s="9"/>
-      <c r="S47" s="9"/>
-      <c r="T47" s="9"/>
-      <c r="U47" s="9"/>
-      <c r="V47" s="9"/>
-      <c r="W47" s="9"/>
-      <c r="X47" s="9"/>
-      <c r="Y47" s="9"/>
-      <c r="Z47" s="9"/>
-      <c r="AA47" s="9"/>
-      <c r="AB47" s="9"/>
-      <c r="AC47" s="9"/>
-      <c r="AD47" s="9"/>
-      <c r="AE47" s="9"/>
-      <c r="AF47" s="9"/>
-      <c r="AG47" s="9"/>
-      <c r="AH47" s="9"/>
-      <c r="AI47" s="9"/>
-      <c r="AJ47" s="9"/>
-      <c r="AK47" s="9"/>
-      <c r="AL47" s="9"/>
-      <c r="AM47" s="9"/>
-      <c r="AN47" s="9"/>
-      <c r="AO47" s="9"/>
-      <c r="AP47" s="9"/>
-      <c r="AQ47" s="9"/>
-      <c r="AR47" s="9"/>
-      <c r="AS47" s="9"/>
-      <c r="AT47" s="9"/>
-      <c r="AU47" s="9"/>
-      <c r="AV47" s="9"/>
-      <c r="AW47" s="9"/>
-      <c r="AX47" s="9"/>
-      <c r="AY47" s="9"/>
-      <c r="AZ47" s="9"/>
-      <c r="BA47" s="9"/>
-      <c r="BB47" s="9"/>
-      <c r="BC47" s="9"/>
-      <c r="BD47" s="9"/>
-      <c r="BE47" s="9"/>
-      <c r="BF47" s="9"/>
-      <c r="BG47" s="9"/>
-      <c r="BH47" s="9"/>
-      <c r="BI47" s="9"/>
-      <c r="BJ47" s="9"/>
-      <c r="BK47" s="9"/>
-      <c r="BL47" s="9"/>
-      <c r="BM47" s="9"/>
-      <c r="BN47" s="9"/>
-      <c r="BO47" s="9"/>
-      <c r="BP47" s="9"/>
-      <c r="BQ47" s="9"/>
-      <c r="BR47" s="9"/>
-      <c r="BS47" s="9"/>
-      <c r="BT47" s="9"/>
-      <c r="BU47" s="9"/>
-      <c r="BV47" s="9"/>
-      <c r="BW47" s="9"/>
-      <c r="BX47" s="9"/>
-      <c r="BY47" s="9"/>
-      <c r="BZ47" s="9"/>
-      <c r="CA47" s="9"/>
-      <c r="CB47" s="9"/>
+      <c r="A47" s="33"/>
+      <c r="B47" s="33"/>
+      <c r="C47" s="33"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+      <c r="N47" s="6"/>
+      <c r="O47" s="6"/>
+      <c r="P47" s="6"/>
+      <c r="Q47" s="6"/>
+      <c r="R47" s="6"/>
+      <c r="S47" s="6"/>
+      <c r="T47" s="6"/>
+      <c r="U47" s="6"/>
+      <c r="V47" s="6"/>
+      <c r="W47" s="6"/>
+      <c r="X47" s="6"/>
+      <c r="Y47" s="6"/>
+      <c r="Z47" s="6"/>
+      <c r="AA47" s="6"/>
+      <c r="AB47" s="6"/>
+      <c r="AC47" s="6"/>
+      <c r="AD47" s="6"/>
+      <c r="AE47" s="6"/>
+      <c r="AF47" s="6"/>
+      <c r="AG47" s="6"/>
+      <c r="AH47" s="6"/>
+      <c r="AI47" s="6"/>
+      <c r="AJ47" s="6"/>
+      <c r="AK47" s="6"/>
+      <c r="AL47" s="6"/>
+      <c r="AM47" s="6"/>
+      <c r="AN47" s="6"/>
+      <c r="AO47" s="6"/>
+      <c r="AP47" s="6"/>
+      <c r="AQ47" s="6"/>
+      <c r="AR47" s="6"/>
+      <c r="AS47" s="6"/>
+      <c r="AT47" s="6"/>
+      <c r="AU47" s="6"/>
+      <c r="AV47" s="6"/>
+      <c r="AW47" s="6"/>
+      <c r="AX47" s="6"/>
+      <c r="AY47" s="6"/>
+      <c r="AZ47" s="6"/>
+      <c r="BA47" s="6"/>
+      <c r="BB47" s="6"/>
+      <c r="BC47" s="6"/>
+      <c r="BD47" s="6"/>
+      <c r="BE47" s="6"/>
+      <c r="BF47" s="6"/>
+      <c r="BG47" s="6"/>
+      <c r="BH47" s="6"/>
+      <c r="BI47" s="6"/>
+      <c r="BJ47" s="6"/>
+      <c r="BK47" s="6"/>
+      <c r="BL47" s="6"/>
+      <c r="BM47" s="6"/>
+      <c r="BN47" s="6"/>
+      <c r="BO47" s="6"/>
+      <c r="BP47" s="6"/>
+      <c r="BQ47" s="6"/>
+      <c r="BR47" s="6"/>
+      <c r="BS47" s="6"/>
+      <c r="BT47" s="6"/>
+      <c r="BU47" s="6"/>
+      <c r="BV47" s="6"/>
+      <c r="BW47" s="6"/>
+      <c r="BX47" s="6"/>
+      <c r="BY47" s="6"/>
+      <c r="BZ47" s="6"/>
+      <c r="CA47" s="6"/>
+      <c r="CB47" s="6"/>
       <c r="CC47" s="6"/>
       <c r="CD47" s="6"/>
       <c r="CE47" s="6"/>
@@ -6854,9 +6774,7 @@
       <c r="DG49" s="6"/>
     </row>
     <row r="50" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
-        <v>47</v>
-      </c>
+      <c r="A50" s="8"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
@@ -7082,10 +7000,8 @@
       <c r="DG51" s="6"/>
     </row>
     <row r="52" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A52" s="10"/>
-      <c r="B52" s="8" t="s">
-        <v>48</v>
-      </c>
+      <c r="A52" s="6"/>
+      <c r="B52" s="8"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
@@ -7310,10 +7226,8 @@
       <c r="DG53" s="6"/>
     </row>
     <row r="54" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A54" s="9"/>
-      <c r="B54" s="8" t="s">
-        <v>49</v>
-      </c>
+      <c r="A54" s="6"/>
+      <c r="B54" s="8"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
@@ -7538,10 +7452,8 @@
       <c r="DG55" s="6"/>
     </row>
     <row r="56" spans="1:111" x14ac:dyDescent="0.25">
-      <c r="A56" s="11"/>
-      <c r="B56" s="8" t="s">
-        <v>50</v>
-      </c>
+      <c r="A56" s="6"/>
+      <c r="B56" s="8"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
@@ -19631,16 +19543,252 @@
       <c r="DG162" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="274">
-    <mergeCell ref="BU8:BW8"/>
-    <mergeCell ref="BX8:BZ8"/>
-    <mergeCell ref="CA8:CC8"/>
-    <mergeCell ref="CD8:CF8"/>
-    <mergeCell ref="BF8:BH8"/>
-    <mergeCell ref="BI8:BK8"/>
-    <mergeCell ref="BL8:BN8"/>
-    <mergeCell ref="BO8:BQ8"/>
-    <mergeCell ref="BR8:BT8"/>
+  <mergeCells count="278">
+    <mergeCell ref="BW37:CA37"/>
+    <mergeCell ref="BW38:CA38"/>
+    <mergeCell ref="BW39:CA39"/>
+    <mergeCell ref="BW40:CA40"/>
+    <mergeCell ref="BW41:CA41"/>
+    <mergeCell ref="BW42:CA42"/>
+    <mergeCell ref="AB24:AF24"/>
+    <mergeCell ref="AE25:AI25"/>
+    <mergeCell ref="AI26:AP26"/>
+    <mergeCell ref="AI29:AJ29"/>
+    <mergeCell ref="AL30:AU30"/>
+    <mergeCell ref="AL31:AZ31"/>
+    <mergeCell ref="BD32:BW32"/>
+    <mergeCell ref="AZ33:BI33"/>
+    <mergeCell ref="BW36:CA36"/>
+    <mergeCell ref="AQ26:AX26"/>
+    <mergeCell ref="AY26:BF26"/>
+    <mergeCell ref="BG26:BN26"/>
+    <mergeCell ref="BO26:BV26"/>
+    <mergeCell ref="P11:V11"/>
+    <mergeCell ref="P12:V12"/>
+    <mergeCell ref="Q15:V15"/>
+    <mergeCell ref="Q16:V16"/>
+    <mergeCell ref="N19:R19"/>
+    <mergeCell ref="N20:R20"/>
+    <mergeCell ref="U21:Y21"/>
+    <mergeCell ref="U22:Y22"/>
+    <mergeCell ref="U23:Y23"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="G1:AH1"/>
+    <mergeCell ref="AI1:BM1"/>
+    <mergeCell ref="BN1:CF1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="BK4:BL4"/>
+    <mergeCell ref="BM4:BN4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AW4:AX4"/>
+    <mergeCell ref="AY4:AZ4"/>
+    <mergeCell ref="BA4:BB4"/>
+    <mergeCell ref="BC4:BD4"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AM4:AN4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AQ4:AR4"/>
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="BY4:BZ4"/>
+    <mergeCell ref="CA4:CB4"/>
+    <mergeCell ref="CC4:CD4"/>
+    <mergeCell ref="CE4:CF4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="BO4:BP4"/>
+    <mergeCell ref="BQ4:BR4"/>
+    <mergeCell ref="BS4:BT4"/>
+    <mergeCell ref="BU4:BV4"/>
+    <mergeCell ref="BW4:BX4"/>
+    <mergeCell ref="BE4:BF4"/>
+    <mergeCell ref="BG4:BH4"/>
+    <mergeCell ref="BI4:BJ4"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="AS5:AT5"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="AW5:AX5"/>
+    <mergeCell ref="AY5:AZ5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="CA5:CB5"/>
+    <mergeCell ref="CC5:CD5"/>
+    <mergeCell ref="BK5:BL5"/>
+    <mergeCell ref="BM5:BN5"/>
+    <mergeCell ref="BO5:BP5"/>
+    <mergeCell ref="BQ5:BR5"/>
+    <mergeCell ref="BS5:BT5"/>
+    <mergeCell ref="BA5:BB5"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="BE5:BF5"/>
+    <mergeCell ref="BG5:BH5"/>
+    <mergeCell ref="BI5:BJ5"/>
+    <mergeCell ref="AM6:AN6"/>
+    <mergeCell ref="AO6:AP6"/>
+    <mergeCell ref="AQ6:AR6"/>
+    <mergeCell ref="AS6:AT6"/>
+    <mergeCell ref="AU6:AV6"/>
+    <mergeCell ref="CE5:CF5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="AG6:AH6"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="AK6:AL6"/>
+    <mergeCell ref="BU5:BV5"/>
+    <mergeCell ref="BW5:BX5"/>
+    <mergeCell ref="BY5:BZ5"/>
+    <mergeCell ref="BI6:BJ6"/>
+    <mergeCell ref="BK6:BL6"/>
+    <mergeCell ref="BM6:BN6"/>
+    <mergeCell ref="BO6:BP6"/>
+    <mergeCell ref="AW6:AX6"/>
+    <mergeCell ref="AY6:AZ6"/>
+    <mergeCell ref="BA6:BB6"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="BE6:BF6"/>
+    <mergeCell ref="BI7:BK7"/>
+    <mergeCell ref="BL7:BN7"/>
+    <mergeCell ref="CA6:CB6"/>
+    <mergeCell ref="CC6:CD6"/>
+    <mergeCell ref="CE6:CF6"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="V7:X7"/>
+    <mergeCell ref="Y7:AA7"/>
+    <mergeCell ref="AB7:AD7"/>
+    <mergeCell ref="AE7:AG7"/>
+    <mergeCell ref="AH7:AJ7"/>
+    <mergeCell ref="AK7:AM7"/>
+    <mergeCell ref="AN7:AP7"/>
+    <mergeCell ref="AQ7:AS7"/>
+    <mergeCell ref="AT7:AV7"/>
+    <mergeCell ref="AW7:AY7"/>
+    <mergeCell ref="BQ6:BR6"/>
+    <mergeCell ref="BS6:BT6"/>
+    <mergeCell ref="BU6:BV6"/>
+    <mergeCell ref="BW6:BX6"/>
+    <mergeCell ref="BY6:BZ6"/>
+    <mergeCell ref="BG6:BH6"/>
     <mergeCell ref="CD7:CF7"/>
     <mergeCell ref="M8:O8"/>
     <mergeCell ref="P8:R8"/>
@@ -19665,247 +19813,15 @@
     <mergeCell ref="AZ7:BB7"/>
     <mergeCell ref="BC7:BE7"/>
     <mergeCell ref="BF7:BH7"/>
-    <mergeCell ref="BI7:BK7"/>
-    <mergeCell ref="BL7:BN7"/>
-    <mergeCell ref="CA6:CB6"/>
-    <mergeCell ref="CC6:CD6"/>
-    <mergeCell ref="CE6:CF6"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="V7:X7"/>
-    <mergeCell ref="Y7:AA7"/>
-    <mergeCell ref="AB7:AD7"/>
-    <mergeCell ref="AE7:AG7"/>
-    <mergeCell ref="AH7:AJ7"/>
-    <mergeCell ref="AK7:AM7"/>
-    <mergeCell ref="AN7:AP7"/>
-    <mergeCell ref="AQ7:AS7"/>
-    <mergeCell ref="AT7:AV7"/>
-    <mergeCell ref="AW7:AY7"/>
-    <mergeCell ref="BQ6:BR6"/>
-    <mergeCell ref="BS6:BT6"/>
-    <mergeCell ref="BU6:BV6"/>
-    <mergeCell ref="BW6:BX6"/>
-    <mergeCell ref="BY6:BZ6"/>
-    <mergeCell ref="BG6:BH6"/>
-    <mergeCell ref="BI6:BJ6"/>
-    <mergeCell ref="BK6:BL6"/>
-    <mergeCell ref="BM6:BN6"/>
-    <mergeCell ref="BO6:BP6"/>
-    <mergeCell ref="AW6:AX6"/>
-    <mergeCell ref="AY6:AZ6"/>
-    <mergeCell ref="BA6:BB6"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="BE6:BF6"/>
-    <mergeCell ref="AM6:AN6"/>
-    <mergeCell ref="AO6:AP6"/>
-    <mergeCell ref="AQ6:AR6"/>
-    <mergeCell ref="AS6:AT6"/>
-    <mergeCell ref="AU6:AV6"/>
-    <mergeCell ref="CE5:CF5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="AG6:AH6"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="AK6:AL6"/>
-    <mergeCell ref="BU5:BV5"/>
-    <mergeCell ref="BW5:BX5"/>
-    <mergeCell ref="BY5:BZ5"/>
-    <mergeCell ref="CA5:CB5"/>
-    <mergeCell ref="CC5:CD5"/>
-    <mergeCell ref="BK5:BL5"/>
-    <mergeCell ref="BM5:BN5"/>
-    <mergeCell ref="BO5:BP5"/>
-    <mergeCell ref="BQ5:BR5"/>
-    <mergeCell ref="BS5:BT5"/>
-    <mergeCell ref="BA5:BB5"/>
-    <mergeCell ref="BC5:BD5"/>
-    <mergeCell ref="BE5:BF5"/>
-    <mergeCell ref="BG5:BH5"/>
-    <mergeCell ref="BI5:BJ5"/>
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="AS5:AT5"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="AW5:AX5"/>
-    <mergeCell ref="AY5:AZ5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="BY4:BZ4"/>
-    <mergeCell ref="CA4:CB4"/>
-    <mergeCell ref="CC4:CD4"/>
-    <mergeCell ref="CE4:CF4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="BO4:BP4"/>
-    <mergeCell ref="BQ4:BR4"/>
-    <mergeCell ref="BS4:BT4"/>
-    <mergeCell ref="BU4:BV4"/>
-    <mergeCell ref="BW4:BX4"/>
-    <mergeCell ref="BE4:BF4"/>
-    <mergeCell ref="BG4:BH4"/>
-    <mergeCell ref="BI4:BJ4"/>
-    <mergeCell ref="BK4:BL4"/>
-    <mergeCell ref="BM4:BN4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AW4:AX4"/>
-    <mergeCell ref="AY4:AZ4"/>
-    <mergeCell ref="BA4:BB4"/>
-    <mergeCell ref="BC4:BD4"/>
-    <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AM4:AN4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AQ4:AR4"/>
-    <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="G1:AH1"/>
-    <mergeCell ref="AI1:BM1"/>
-    <mergeCell ref="BN1:CF1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="P11:V11"/>
-    <mergeCell ref="P12:V12"/>
-    <mergeCell ref="Q15:V15"/>
-    <mergeCell ref="Q16:V16"/>
-    <mergeCell ref="N19:R19"/>
-    <mergeCell ref="N20:R20"/>
-    <mergeCell ref="U21:Y21"/>
-    <mergeCell ref="U22:Y22"/>
-    <mergeCell ref="U23:Y23"/>
-    <mergeCell ref="BW37:CA37"/>
-    <mergeCell ref="BW38:CA38"/>
-    <mergeCell ref="BW39:CA39"/>
-    <mergeCell ref="BW40:CA40"/>
-    <mergeCell ref="BW41:CA41"/>
-    <mergeCell ref="BW42:CA42"/>
-    <mergeCell ref="AB24:AF24"/>
-    <mergeCell ref="AE25:AI25"/>
-    <mergeCell ref="AI26:AP26"/>
-    <mergeCell ref="AI29:AJ29"/>
-    <mergeCell ref="AL30:AU30"/>
-    <mergeCell ref="AL31:AZ31"/>
-    <mergeCell ref="BD32:BW32"/>
-    <mergeCell ref="AZ33:BI33"/>
-    <mergeCell ref="BW36:CA36"/>
+    <mergeCell ref="BU8:BW8"/>
+    <mergeCell ref="BX8:BZ8"/>
+    <mergeCell ref="CA8:CC8"/>
+    <mergeCell ref="CD8:CF8"/>
+    <mergeCell ref="BF8:BH8"/>
+    <mergeCell ref="BI8:BK8"/>
+    <mergeCell ref="BL8:BN8"/>
+    <mergeCell ref="BO8:BQ8"/>
+    <mergeCell ref="BR8:BT8"/>
   </mergeCells>
   <conditionalFormatting sqref="G4:CF4">
     <cfRule type="colorScale" priority="1">

</xml_diff>